<commit_message>
update shapefile id and metadata description
</commit_message>
<xml_diff>
--- a/SPAM_metadata.xlsx
+++ b/SPAM_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapy\OneDrive - COWI\Data\SPAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0ECD07-6213-46CF-8A5E-F916B02BA43E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="6_{A236FFC5-8F44-4E4A-B63C-6E8C5ECADD87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{8C599A39-ABA7-4E4F-A286-DE24DD7B8148}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5145" yWindow="2880" windowWidth="19185" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SHAPEFILES" sheetId="5" r:id="rId1"/>
@@ -441,16 +441,10 @@
     <t>Countries_WGS84</t>
   </si>
   <si>
-    <t>ncatch</t>
-  </si>
-  <si>
     <t>ncountry</t>
   </si>
   <si>
     <t>nshape</t>
-  </si>
-  <si>
-    <t>nshape: index of shapefiles, used as name for outputs</t>
   </si>
   <si>
     <t>SPAM data reader - SHAPEFILES information</t>
@@ -755,6 +749,12 @@
   </si>
   <si>
     <t>It is usefull if the output files are disclosed from this option file</t>
+  </si>
+  <si>
+    <t>nshape: index of shapefiles will appear in output file names</t>
+  </si>
+  <si>
+    <t>ncatch</t>
   </si>
 </sst>
 </file>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07E633F-D53A-486A-A220-D4B01B3A87A7}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -1113,12 +1113,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>137</v>
+        <v>203</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1170,13 +1170,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
@@ -1187,7 +1187,7 @@
         <v>132</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
@@ -1198,7 +1198,7 @@
         <v>133</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1211,7 +1211,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -1227,12 +1227,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1295,22 +1295,22 @@
         <v>128</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>123</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
@@ -1337,10 +1337,10 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
@@ -1370,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -1397,10 +1397,10 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -1427,10 +1427,10 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1462,12 +1462,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -1521,7 +1521,7 @@
         <v>108</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -2136,12 +2136,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2149,7 +2149,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2157,7 +2157,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2173,12 +2173,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -2195,7 +2195,7 @@
         <v>122</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
@@ -2247,7 +2247,7 @@
         <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2284,12 +2284,12 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2305,7 +2305,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2533,7 +2533,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:E16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -2543,12 +2543,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2556,7 +2556,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2580,12 +2580,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -2596,23 +2596,23 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2636,10 +2636,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2651,7 +2651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BBD5C0-1DC9-4756-B764-615EFB75BD9E}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2659,7 +2659,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -2670,7 +2670,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2704,34 +2704,34 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
@@ -2739,7 +2739,7 @@
         <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -2747,7 +2747,7 @@
         <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
@@ -2755,7 +2755,7 @@
         <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2765,12 +2765,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2944,15 +2941,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F7C223-802B-42EB-B5C2-D3FF359503BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E40BF96-B965-4FD2-ACE9-AF8318D4C022}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a6ec2889-8209-4b3f-8525-703b317acf75"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2976,17 +2984,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E40BF96-B965-4FD2-ACE9-AF8318D4C022}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F7C223-802B-42EB-B5C2-D3FF359503BB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a6ec2889-8209-4b3f-8525-703b317acf75"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>